<commit_message>
- Update recipes for Short Question - Import DYSaC short questions - Add column to spreadsheet for Trait
</commit_message>
<xml_diff>
--- a/GetJobProfiles/SeedData/dysac.xlsx
+++ b/GetJobProfiles/SeedData/dysac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\dfc-servicetaxonomy-editor\GetJobProfiles\SeedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3E8D13-64D9-4A1F-95A6-232F393D3FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD863EFC-8456-47B4-8DD5-F3F79F8B2AB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="21600" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shortquestion" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="724">
   <si>
     <t>SystemParentId</t>
   </si>
@@ -2192,6 +2192,9 @@
   </si>
   <si>
     <t>endurance</t>
+  </si>
+  <si>
+    <t>Trait</t>
   </si>
 </sst>
 </file>
@@ -3034,9 +3037,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -3067,7 +3082,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -3099,7 +3114,7 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -3131,7 +3146,7 @@
         <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -3163,7 +3178,7 @@
         <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -3195,7 +3210,7 @@
         <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -3227,7 +3242,7 @@
         <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -3259,7 +3274,7 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -3291,7 +3306,7 @@
         <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -3323,7 +3338,7 @@
         <v>50</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -3355,7 +3370,7 @@
         <v>55</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -3387,7 +3402,7 @@
         <v>60</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -3419,7 +3434,7 @@
         <v>65</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -3451,7 +3466,7 @@
         <v>69</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -3483,7 +3498,7 @@
         <v>74</v>
       </c>
       <c r="J14" t="s">
-        <v>17</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -3515,7 +3530,7 @@
         <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -3547,7 +3562,7 @@
         <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -3579,7 +3594,7 @@
         <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -3611,7 +3626,7 @@
         <v>91</v>
       </c>
       <c r="J18" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -3643,7 +3658,7 @@
         <v>95</v>
       </c>
       <c r="J19" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -3675,7 +3690,7 @@
         <v>99</v>
       </c>
       <c r="J20" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -3707,7 +3722,7 @@
         <v>104</v>
       </c>
       <c r="J21" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
@@ -3739,7 +3754,7 @@
         <v>108</v>
       </c>
       <c r="J22" t="s">
-        <v>17</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
@@ -3771,7 +3786,7 @@
         <v>112</v>
       </c>
       <c r="J23" t="s">
-        <v>17</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -3803,7 +3818,7 @@
         <v>116</v>
       </c>
       <c r="J24" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -3835,7 +3850,7 @@
         <v>121</v>
       </c>
       <c r="J25" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -3867,7 +3882,7 @@
         <v>126</v>
       </c>
       <c r="J26" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -3899,7 +3914,7 @@
         <v>132</v>
       </c>
       <c r="J27" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -3931,7 +3946,7 @@
         <v>136</v>
       </c>
       <c r="J28" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -3963,7 +3978,7 @@
         <v>141</v>
       </c>
       <c r="J29" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -3995,7 +4010,7 @@
         <v>145</v>
       </c>
       <c r="J30" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -4027,7 +4042,7 @@
         <v>150</v>
       </c>
       <c r="J31" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -4059,7 +4074,7 @@
         <v>155</v>
       </c>
       <c r="J32" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -4091,7 +4106,7 @@
         <v>159</v>
       </c>
       <c r="J33" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -4123,7 +4138,7 @@
         <v>163</v>
       </c>
       <c r="J34" t="s">
-        <v>17</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -4155,7 +4170,7 @@
         <v>167</v>
       </c>
       <c r="J35" t="s">
-        <v>17</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -4187,7 +4202,7 @@
         <v>171</v>
       </c>
       <c r="J36" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -4219,7 +4234,7 @@
         <v>175</v>
       </c>
       <c r="J37" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -4251,7 +4266,7 @@
         <v>179</v>
       </c>
       <c r="J38" t="s">
-        <v>17</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -4283,7 +4298,7 @@
         <v>183</v>
       </c>
       <c r="J39" t="s">
-        <v>17</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -4315,7 +4330,7 @@
         <v>187</v>
       </c>
       <c r="J40" t="s">
-        <v>17</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -4347,7 +4362,7 @@
         <v>192</v>
       </c>
       <c r="J41" t="s">
-        <v>17</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -4764,9 +4779,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="10" max="10" width="48.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>